<commit_message>
fix best run MAG9
</commit_message>
<xml_diff>
--- a/DESMAN/DESMAN_other_MAGs/desman_results.xlsx
+++ b/DESMAN/DESMAN_other_MAGs/desman_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>MAG10_6_6</t>
   </si>
   <si>
-    <t>MAG9_7_9</t>
-  </si>
-  <si>
     <t>MAG8_11_4</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>MAG9_7_1</t>
   </si>
 </sst>
 </file>
@@ -414,17 +414,17 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,21 +432,21 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -458,12 +458,12 @@
         <v>2.5420532548800001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -475,12 +475,12 @@
         <v>4.3052272130300002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -492,12 +492,12 @@
         <v>2.0900444853500001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -509,12 +509,12 @@
         <v>3.6297868993999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -526,12 +526,12 @@
         <v>5.6353902507699997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -543,12 +543,12 @@
         <v>1.25987430087E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -560,12 +560,12 @@
         <v>2.1017366744799999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>11</v>
@@ -577,12 +577,12 @@
         <v>4.27890684732E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -594,7 +594,7 @@
         <v>2.78657035414E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>10</v>
       </c>

</xml_diff>